<commit_message>
Modificación matriz de trazabilidad de reglas de negocio
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RN.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\UNI\2º\IISSI-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\UNI\2º\IISSI-1\svn\repos\deporte_y_desafio\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED6F864-10DD-4C8D-8DA5-FE0055125D89}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A346E7A0-5A31-452C-96A7-05482CBC4C9B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Participante</t>
   </si>
   <si>
-    <t>C/A                           R</t>
-  </si>
-  <si>
     <t>Mensaje</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Pregunta</t>
+  </si>
+  <si>
+    <t>A                           RN</t>
   </si>
 </sst>
 </file>
@@ -851,6 +851,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,10 +935,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -881,89 +953,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,103 +1335,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="36"/>
       <c r="C1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
       <c r="O2" s="28"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
     </row>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1439,11 +1439,11 @@
       <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="45"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1454,18 +1454,18 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="9"/>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1479,15 +1479,15 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="44"/>
+      <c r="A6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1497,7 +1497,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1505,10 +1505,10 @@
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1521,18 +1521,18 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1546,15 +1546,15 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="20"/>
+      <c r="A9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="21"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1567,20 +1567,20 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="20"/>
+      <c r="A10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="21"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1595,10 +1595,10 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="20"/>
+      <c r="A11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="21"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1611,23 +1611,23 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="20"/>
+      <c r="A12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="21"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1639,10 +1639,10 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="40"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1654,55 +1654,55 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="20"/>
+      <c r="A15" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="21"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1715,62 +1715,62 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="A16" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="40"/>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="20"/>
+      <c r="A17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="21"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1785,14 +1785,14 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="20"/>
+      <c r="A18" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="21"/>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1805,16 +1805,16 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1826,17 +1826,17 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="20"/>
+      <c r="A20" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="21"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1851,19 +1851,19 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="18"/>
+      <c r="A21" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="40"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1871,22 +1871,22 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="24"/>
+      <c r="A22" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="42"/>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1901,14 +1901,14 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="26"/>
+      <c r="A23" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="44"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -1916,22 +1916,22 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -1945,26 +1945,10 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
@@ -1978,12 +1962,28 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1995,101 +1995,101 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B1" s="54"/>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="E1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="F1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="G1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="H1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="I1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="J1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="L1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="M1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="O1" s="47" t="s">
         <v>34</v>
-      </c>
-      <c r="O1" s="49" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="55"/>
       <c r="B2" s="56"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="52"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="46"/>
+      <c r="A3" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="50"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="48"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="24"/>
+      <c r="A4" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="42"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2097,10 +2097,10 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -2109,10 +2109,10 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="18"/>
+      <c r="A5" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="40"/>
       <c r="C5" s="6"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2128,10 +2128,10 @@
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="20"/>
+      <c r="A6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="21"/>
       <c r="C6" s="6"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2141,7 +2141,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2149,10 +2149,10 @@
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="20"/>
+      <c r="A7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="21"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2165,15 +2165,15 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="20"/>
+      <c r="A8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2189,10 +2189,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="18"/>
+      <c r="A9" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="40"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2203,23 +2203,23 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="20"/>
+      <c r="A10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="21"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2231,10 +2231,10 @@
       <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="18"/>
+      <c r="A11" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="40"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2246,16 +2246,16 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="20"/>
+      <c r="A12" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="21"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2271,10 +2271,10 @@
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="22"/>
+      <c r="A13" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="46"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2290,10 +2290,10 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="40"/>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2309,14 +2309,14 @@
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="20"/>
+      <c r="A15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="21"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2330,10 +2330,10 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="A16" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="40"/>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2349,10 +2349,10 @@
       <c r="O16" s="9"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="A17" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="40"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2368,18 +2368,18 @@
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="18"/>
+      <c r="A18" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="40"/>
       <c r="C18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2393,10 +2393,10 @@
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="24"/>
+      <c r="A19" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="42"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2407,22 +2407,22 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="24"/>
+      <c r="A20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="42"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2435,17 +2435,17 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="26"/>
+      <c r="A21" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="44"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2456,28 +2456,46 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42" t="s">
-        <v>36</v>
+      <c r="A22" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A22:B22"/>
@@ -2494,24 +2512,6 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de la matriz de trazabilidad de reglas de negocio
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RN.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\UNI\2º\IISSI-1\svn\repos\deporte_y_desafio\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A346E7A0-5A31-452C-96A7-05482CBC4C9B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110CC63A-E0D9-47E0-B305-663F5AF76125}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="56">
   <si>
     <t>Actividad</t>
   </si>
@@ -872,12 +872,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,64 +941,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,36 +982,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,82 +1335,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
     </row>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
@@ -1439,10 +1439,10 @@
       <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="17"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1461,10 +1461,10 @@
       <c r="P4" s="9"/>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1483,10 +1483,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="16"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1505,10 +1505,10 @@
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1529,10 +1529,10 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1551,10 +1551,10 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1573,10 +1573,10 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -1595,10 +1595,10 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1617,10 +1617,10 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1639,10 +1639,10 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="40"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1661,10 +1661,10 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
@@ -1699,10 +1699,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1721,10 +1721,10 @@
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
@@ -1756,21 +1756,17 @@
       <c r="M16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1789,10 +1785,10 @@
       </c>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1811,10 +1807,10 @@
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1833,10 +1829,10 @@
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1855,10 +1851,10 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="40"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1883,10 +1879,10 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1905,10 +1901,10 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -1945,6 +1941,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
@@ -1961,29 +1980,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2001,72 +1997,72 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="45" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="3"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -2086,10 +2082,10 @@
       <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="42"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2109,10 +2105,10 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="6"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2128,10 +2124,10 @@
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="6"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2149,10 +2145,10 @@
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2170,10 +2166,10 @@
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2189,10 +2185,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="40"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2210,10 +2206,10 @@
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2231,10 +2227,10 @@
       <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2252,10 +2248,10 @@
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2271,10 +2267,10 @@
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="46"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2290,10 +2286,10 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2309,10 +2305,10 @@
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
@@ -2330,10 +2326,10 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2349,10 +2345,10 @@
       <c r="O16" s="9"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="40"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2368,10 +2364,10 @@
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
@@ -2393,10 +2389,10 @@
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2414,10 +2410,10 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="42"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2435,10 +2431,10 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="44"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2456,10 +2452,10 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -2478,24 +2474,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A22:B22"/>
@@ -2512,6 +2490,24 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios añadidos a matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/documentacion/matriz_de_trazabilidad_RN.xlsx
+++ b/documentacion/matriz_de_trazabilidad_RN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\UNI\2º\IISSI-1\svn\repos\deporte_y_desafio\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC6FECE-1CDC-4A96-ABFD-A0E8463D8C55}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CF4C65-68E8-4956-A9BF-693B22DB790E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="54">
   <si>
     <t>Actividad</t>
   </si>
@@ -69,21 +69,12 @@
     <t>financia</t>
   </si>
   <si>
-    <t>obtiene</t>
-  </si>
-  <si>
-    <t>plantea</t>
-  </si>
-  <si>
     <t>realiza</t>
   </si>
   <si>
     <t>hace</t>
   </si>
   <si>
-    <t>presenta</t>
-  </si>
-  <si>
     <t>recibe</t>
   </si>
   <si>
@@ -187,6 +178,12 @@
   </si>
   <si>
     <t>A                           RN</t>
+  </si>
+  <si>
+    <t>RN-014</t>
+  </si>
+  <si>
+    <t>RN-015</t>
   </si>
 </sst>
 </file>
@@ -210,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -810,11 +807,75 @@
         <color auto="1"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -869,18 +930,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -896,53 +1002,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -950,36 +1044,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1320,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1332,114 +1415,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="31" t="s">
+      <c r="A1" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="G1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="I1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="J1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="M1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="N1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="29" t="s">
+      <c r="O1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="P1" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="Q1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="41"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="36"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="41"/>
     </row>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="8"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="68"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="17"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1451,17 +1543,21 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="9"/>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="21"/>
+      <c r="A5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="26"/>
       <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1475,15 +1571,19 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="9"/>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="21"/>
+      <c r="A6" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="26"/>
       <c r="C6" s="16"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1494,18 +1594,22 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="9"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1518,18 +1622,20 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1543,15 +1649,17 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="9"/>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="21"/>
+      <c r="A9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="26"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1564,20 +1672,22 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="9"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="9"/>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="21"/>
+      <c r="A10" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1589,13 +1699,15 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="9"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="21"/>
+      <c r="A11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="26"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1608,23 +1720,27 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="9"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="9"/>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="21"/>
+      <c r="A12" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="26"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1633,13 +1749,15 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="9"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="9"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1651,55 +1769,64 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="9"/>
+      <c r="P13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="P14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" s="68"/>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1712,58 +1839,62 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O15" s="2"/>
-      <c r="P15" s="9"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="23"/>
+      <c r="A16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="34"/>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="21"/>
+      <c r="P16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="9"/>
+    </row>
+    <row r="17" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="26"/>
       <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1777,15 +1908,17 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="21"/>
+      <c r="P17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="9"/>
+    </row>
+    <row r="18" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="26"/>
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1798,19 +1931,23 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="9"/>
-    </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="22" t="s">
+      <c r="P18" s="2"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="59"/>
+    </row>
+    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1819,17 +1956,21 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="9"/>
-    </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="21"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" s="63"/>
+    </row>
+    <row r="20" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="26"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1843,20 +1984,22 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="22" t="s">
+      <c r="P20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q20" s="60"/>
+      <c r="R20" s="64"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1864,22 +2007,24 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="37" t="s">
+      <c r="P21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="63"/>
+    </row>
+    <row r="22" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="38"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1893,15 +2038,17 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="39" t="s">
+      <c r="P22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="64"/>
+    </row>
+    <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -1909,35 +2056,65 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="P23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R24" s="65"/>
+    </row>
+    <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A10:B10"/>
@@ -1953,30 +2130,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1985,81 +2138,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="47" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="I1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="J1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="K1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="M1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="N1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="O1" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="50"/>
+      <c r="P1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="66"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="55"/>
       <c r="C3" s="3"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -2067,22 +2228,26 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
-      <c r="O3" s="19"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="37" t="s">
+      <c r="O3" s="18"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2090,22 +2255,26 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="22" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="6"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2118,13 +2287,17 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="21"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="26"/>
       <c r="C6" s="6"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2134,18 +2307,22 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="21"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="26"/>
       <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2158,15 +2335,17 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="21"/>
+        <v>32</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="26"/>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2179,13 +2358,17 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="22" t="s">
+      <c r="O8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2196,17 +2379,19 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="22" t="s">
+      <c r="O9" s="2"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2218,19 +2403,25 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="21"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="9"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="26"/>
       <c r="C11" s="6"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2240,13 +2431,15 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="46"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="57"/>
       <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2259,16 +2452,20 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="23"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="26"/>
       <c r="C13" s="6"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2277,18 +2474,26 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2299,13 +2504,17 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="23"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="22"/>
       <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2315,21 +2524,31 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="23"/>
+      <c r="O15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="22"/>
       <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2337,121 +2556,79 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="9"/>
+    </row>
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="9"/>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="15" t="s">
-        <v>35</v>
-      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="9"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="32">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="H1:H2"/>
@@ -2463,28 +2640,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>